<commit_message>
update upload contract and add contractlist module testcases
</commit_message>
<xml_diff>
--- a/TestData/test_data.xlsx
+++ b/TestData/test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22530" windowHeight="8265" firstSheet="1" activeTab="7"/>
+    <workbookView windowWidth="19284" windowHeight="8555" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="reset_psw" sheetId="3" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="sql_data" sheetId="8" r:id="rId6"/>
     <sheet name="code_login" sheetId="9" r:id="rId7"/>
     <sheet name="upload_contract" sheetId="10" r:id="rId8"/>
+    <sheet name="contract_list" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="146">
   <si>
     <t>phone</t>
   </si>
@@ -436,6 +437,30 @@
   </si>
   <si>
     <t>上传错误格式</t>
+  </si>
+  <si>
+    <t>bss</t>
+  </si>
+  <si>
+    <t>哈哈哈</t>
+  </si>
+  <si>
+    <t>没有数据哦~</t>
+  </si>
+  <si>
+    <t>搜索文档无数据</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>拒绝契约，拒绝契约</t>
+  </si>
+  <si>
+    <t>操作成功</t>
+  </si>
+  <si>
+    <t>拒绝原因不能为空</t>
   </si>
 </sst>
 </file>
@@ -443,9 +468,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -458,32 +483,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -501,47 +503,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,7 +521,53 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -571,16 +581,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -588,7 +590,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -600,6 +602,29 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -610,31 +635,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -646,19 +791,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -670,127 +803,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -804,17 +829,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -823,16 +859,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -856,48 +898,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -909,10 +934,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -921,133 +946,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1386,11 +1411,11 @@
       <selection activeCell="A8" sqref="$A8:$XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="19.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="1" max="1" width="19.6296296296296" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.6296296296296" customWidth="1"/>
+    <col min="3" max="3" width="23.1296296296296" customWidth="1"/>
     <col min="4" max="4" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1508,12 +1533,12 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.1296296296296" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="32.375" customWidth="1"/>
+    <col min="4" max="4" width="32.3796296296296" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1766,12 +1791,12 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="13.25"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="17.1296296296296" customWidth="1"/>
+    <col min="3" max="3" width="18.8796296296296" customWidth="1"/>
+    <col min="4" max="4" width="31.8796296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1907,11 +1932,11 @@
       <selection activeCell="A8" sqref="$A8:$XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="28.75" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
+    <col min="3" max="3" width="32.8796296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2025,12 +2050,12 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="14.75" customWidth="1"/>
     <col min="2" max="2" width="16.25" customWidth="1"/>
-    <col min="3" max="3" width="24.375" customWidth="1"/>
-    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="24.3796296296296" customWidth="1"/>
+    <col min="4" max="4" width="14.6296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2073,12 +2098,12 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="42.375" customWidth="1"/>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="65.375" customWidth="1"/>
+    <col min="1" max="1" width="42.3796296296296" customWidth="1"/>
+    <col min="2" max="2" width="17.6296296296296" customWidth="1"/>
+    <col min="3" max="3" width="16.1296296296296" customWidth="1"/>
+    <col min="4" max="4" width="65.3796296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2264,9 +2289,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.3796296296296" style="2" customWidth="1"/>
     <col min="2" max="2" width="38.25" customWidth="1"/>
     <col min="3" max="3" width="32.75" customWidth="1"/>
   </cols>
@@ -2343,17 +2368,17 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="76.25" customWidth="1"/>
     <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="3" max="3" width="23.125" customWidth="1"/>
+    <col min="3" max="3" width="23.1296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2367,7 +2392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="57" spans="1:3">
+    <row r="2" ht="55.2" spans="1:3">
       <c r="A2" t="s">
         <v>123</v>
       </c>
@@ -2378,7 +2403,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" ht="57" spans="1:3">
+    <row r="3" ht="55.2" spans="1:3">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -2389,7 +2414,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" ht="57" spans="1:3">
+    <row r="4" ht="55.2" spans="1:3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2400,7 +2425,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" ht="57" spans="1:3">
+    <row r="5" ht="55.2" spans="1:3">
       <c r="A5" t="s">
         <v>130</v>
       </c>
@@ -2431,6 +2456,68 @@
       </c>
       <c r="C7" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="13.8" outlineLevelRow="2" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="28.3333333333333" customWidth="1"/>
+    <col min="2" max="2" width="19.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>